<commit_message>
concludes feeds imports script
</commit_message>
<xml_diff>
--- a/groups.xlsx
+++ b/groups.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="790">
   <si>
     <t>GroupID: 324309874271040</t>
   </si>
@@ -2354,6 +2355,36 @@
   </si>
   <si>
     <t>829432750433136</t>
+  </si>
+  <si>
+    <t>MemberID</t>
+  </si>
+  <si>
+    <t>GroupsIDs</t>
+  </si>
+  <si>
+    <t>['324309874271040', '255488514638473', '334271300068285']</t>
+  </si>
+  <si>
+    <t>['324309874271040', '255488514638473']</t>
+  </si>
+  <si>
+    <t>['206494919465453', '255488514638473']</t>
+  </si>
+  <si>
+    <t>['255488514638473', '334271300068285']</t>
+  </si>
+  <si>
+    <t>['324309874271040', '334271300068285']</t>
+  </si>
+  <si>
+    <t>['324309874271040', '206494919465453']</t>
+  </si>
+  <si>
+    <t>['324309874271040', '206494919465453', '255488514638473', '334271300068285']</t>
+  </si>
+  <si>
+    <t>['324309874271040', '206494919465453', '255488514638473']</t>
   </si>
 </sst>
 </file>
@@ -2685,7 +2716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:B521"/>
+  <dimension ref="A3:B522"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6819,6 +6850,888 @@
         <v>239</v>
       </c>
     </row>
+    <row r="522" spans="1:2">
+      <c r="A522">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B108"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B4" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>707</v>
+      </c>
+      <c r="B6" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>653</v>
+      </c>
+      <c r="B10" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>387</v>
+      </c>
+      <c r="B12" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B13" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>403</v>
+      </c>
+      <c r="B16" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>407</v>
+      </c>
+      <c r="B17" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>367</v>
+      </c>
+      <c r="B20" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B26" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>423</v>
+      </c>
+      <c r="B27" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>263</v>
+      </c>
+      <c r="B30" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>333</v>
+      </c>
+      <c r="B31" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>365</v>
+      </c>
+      <c r="B34" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>309</v>
+      </c>
+      <c r="B35" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>393</v>
+      </c>
+      <c r="B36" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>415</v>
+      </c>
+      <c r="B37" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>301</v>
+      </c>
+      <c r="B38" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>375</v>
+      </c>
+      <c r="B39" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>241</v>
+      </c>
+      <c r="B40" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>677</v>
+      </c>
+      <c r="B41" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>405</v>
+      </c>
+      <c r="B42" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>641</v>
+      </c>
+      <c r="B48" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>339</v>
+      </c>
+      <c r="B50" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>397</v>
+      </c>
+      <c r="B53" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>305</v>
+      </c>
+      <c r="B55" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>401</v>
+      </c>
+      <c r="B56" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>313</v>
+      </c>
+      <c r="B57" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>391</v>
+      </c>
+      <c r="B60" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>371</v>
+      </c>
+      <c r="B63" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>283</v>
+      </c>
+      <c r="B64" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>259</v>
+      </c>
+      <c r="B65" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>243</v>
+      </c>
+      <c r="B66" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>409</v>
+      </c>
+      <c r="B70" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>399</v>
+      </c>
+      <c r="B72" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>285</v>
+      </c>
+      <c r="B74" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>427</v>
+      </c>
+      <c r="B75" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>235</v>
+      </c>
+      <c r="B76" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>417</v>
+      </c>
+      <c r="B79" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>281</v>
+      </c>
+      <c r="B80" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>287</v>
+      </c>
+      <c r="B81" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>177</v>
+      </c>
+      <c r="B82" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>691</v>
+      </c>
+      <c r="B84" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>185</v>
+      </c>
+      <c r="B85" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>211</v>
+      </c>
+      <c r="B87" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>329</v>
+      </c>
+      <c r="B88" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>377</v>
+      </c>
+      <c r="B90" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>411</v>
+      </c>
+      <c r="B91" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>171</v>
+      </c>
+      <c r="B93" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>331</v>
+      </c>
+      <c r="B94" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>227</v>
+      </c>
+      <c r="B96" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>381</v>
+      </c>
+      <c r="B97" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>413</v>
+      </c>
+      <c r="B98" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>267</v>
+      </c>
+      <c r="B99" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>431</v>
+      </c>
+      <c r="B100" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>421</v>
+      </c>
+      <c r="B101" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>119</v>
+      </c>
+      <c r="B102" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>175</v>
+      </c>
+      <c r="B103" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>369</v>
+      </c>
+      <c r="B104" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>221</v>
+      </c>
+      <c r="B105" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>345</v>
+      </c>
+      <c r="B107" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>439</v>
+      </c>
+      <c r="B108" t="s">
+        <v>784</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>